<commit_message>
Finalización bot BY MONTH
</commit_message>
<xml_diff>
--- a/bots/bot_B&S/REPS.xlsx
+++ b/bots/bot_B&S/REPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvargasp\Documents\Archivos MAAJI\Otros\UIPath RPA\bot_B&amp;S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7C2226-B3B6-402C-8EE1-4B205C80340D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7C248D-4D8A-4FBF-AFDE-3D9085A949E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A4402FF1-2824-4630-A8A8-175FFB4CDC89}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>